<commit_message>
Attempted more of the add items to cart. not working well.
</commit_message>
<xml_diff>
--- a/Criteria.xlsx
+++ b/Criteria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB0638A-3EBA-4B24-BEE8-73C8A2DC3C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EA6D0E-31C5-46CD-A09C-660671C20245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{49FD44CF-2563-4D17-9CD5-E971B4180E73}"/>
   </bookViews>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F612DAF-6014-4C10-B1BF-66B5D8C0C040}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -583,7 +583,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="102" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -603,7 +603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -623,7 +623,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
@@ -643,7 +643,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="102" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -663,7 +663,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -683,7 +683,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="56.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -701,7 +701,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -719,7 +719,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="56.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -753,7 +753,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
@@ -769,7 +769,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="56.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -785,21 +785,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="56.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="84.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -813,7 +813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -827,7 +827,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -839,7 +839,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="56.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>21</v>
       </c>
@@ -851,7 +851,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="98.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Nathan has saved me with log in.
</commit_message>
<xml_diff>
--- a/Criteria.xlsx
+++ b/Criteria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EA6D0E-31C5-46CD-A09C-660671C20245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF470AC-3900-4898-AE8C-6EA587577FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{49FD44CF-2563-4D17-9CD5-E971B4180E73}"/>
   </bookViews>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F612DAF-6014-4C10-B1BF-66B5D8C0C040}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -684,38 +684,38 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="2" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Got sign up working.Need to add password validation and output that to the user.
</commit_message>
<xml_diff>
--- a/Criteria.xlsx
+++ b/Criteria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF470AC-3900-4898-AE8C-6EA587577FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D9E05D-B4B6-43F1-A8F3-F7EEBD686BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{49FD44CF-2563-4D17-9CD5-E971B4180E73}"/>
   </bookViews>
@@ -557,7 +557,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated readme and Changed welcome message. Css needs sorting.
</commit_message>
<xml_diff>
--- a/Criteria.xlsx
+++ b/Criteria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D9E05D-B4B6-43F1-A8F3-F7EEBD686BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45B5C32-EC49-4203-901B-88D57552EFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{49FD44CF-2563-4D17-9CD5-E971B4180E73}"/>
+    <workbookView xWindow="14310" yWindow="0" windowWidth="14580" windowHeight="17370" xr2:uid="{49FD44CF-2563-4D17-9CD5-E971B4180E73}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F612DAF-6014-4C10-B1BF-66B5D8C0C040}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -720,20 +720,20 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="5" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added conn.php call to top of files.
</commit_message>
<xml_diff>
--- a/Criteria.xlsx
+++ b/Criteria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45B5C32-EC49-4203-901B-88D57552EFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3439C2A6-CB6F-4B42-9AB2-53CFBA97DA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14310" yWindow="0" windowWidth="14580" windowHeight="17370" xr2:uid="{49FD44CF-2563-4D17-9CD5-E971B4180E73}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{49FD44CF-2563-4D17-9CD5-E971B4180E73}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -557,7 +557,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="F12" sqref="A12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -770,18 +770,18 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Got filter's to stay at the top.
</commit_message>
<xml_diff>
--- a/Criteria.xlsx
+++ b/Criteria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3439C2A6-CB6F-4B42-9AB2-53CFBA97DA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B337D8-EB29-4B31-B199-5CD6A0485E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{49FD44CF-2563-4D17-9CD5-E971B4180E73}"/>
   </bookViews>
@@ -557,7 +557,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="A12:F12"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -754,18 +754,18 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="5" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -828,14 +828,14 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3" t="s">
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>